<commit_message>
Changes for part 1
</commit_message>
<xml_diff>
--- a/Retail_Sales_Data.xlsx
+++ b/Retail_Sales_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/89DCEDB2710A58D6/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/015e87c30f626ada/Desktop/IS303/Pandas-PostgreSQL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BEF0B36-7D26-46C1-90D4-FF999DDCFDE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2C4924CC-D04C-4CDF-BD79-9B5E314D848E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1470" windowWidth="21600" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -845,18 +845,18 @@
   <dimension ref="A1:K501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="19.77734375" customWidth="1"/>
-    <col min="5" max="5" width="18.77734375" customWidth="1"/>
+    <col min="2" max="2" width="19.796875" customWidth="1"/>
+    <col min="5" max="5" width="18.796875" customWidth="1"/>
     <col min="6" max="6" width="17.6640625" customWidth="1"/>
     <col min="7" max="9" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>135</v>
       </c>
@@ -891,7 +891,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -926,7 +926,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -961,7 +961,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -996,7 +996,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1031,7 +1031,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1171,7 +1171,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1451,7 +1451,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1696,7 +1696,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1766,7 +1766,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1836,7 +1836,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1871,7 +1871,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2046,7 +2046,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2291,7 +2291,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2396,7 +2396,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2431,7 +2431,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2676,7 +2676,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2746,7 +2746,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2781,7 +2781,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2816,7 +2816,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2886,7 +2886,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2956,7 +2956,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3026,7 +3026,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3061,7 +3061,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3096,7 +3096,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3131,7 +3131,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>66</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3236,7 +3236,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3271,7 +3271,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3306,7 +3306,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3341,7 +3341,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3376,7 +3376,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3411,7 +3411,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3446,7 +3446,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3481,7 +3481,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>77</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A79">
         <v>78</v>
       </c>
@@ -3621,7 +3621,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A80">
         <v>79</v>
       </c>
@@ -3656,7 +3656,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A81">
         <v>80</v>
       </c>
@@ -3691,7 +3691,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A82">
         <v>81</v>
       </c>
@@ -3726,7 +3726,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A83">
         <v>82</v>
       </c>
@@ -3761,7 +3761,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A84">
         <v>83</v>
       </c>
@@ -3796,7 +3796,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A85">
         <v>84</v>
       </c>
@@ -3831,7 +3831,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A86">
         <v>85</v>
       </c>
@@ -3866,7 +3866,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A87">
         <v>86</v>
       </c>
@@ -3901,7 +3901,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A88">
         <v>87</v>
       </c>
@@ -3936,7 +3936,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A89">
         <v>88</v>
       </c>
@@ -3971,7 +3971,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A90">
         <v>89</v>
       </c>
@@ -4006,7 +4006,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A91">
         <v>90</v>
       </c>
@@ -4041,7 +4041,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A92">
         <v>91</v>
       </c>
@@ -4076,7 +4076,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A93">
         <v>92</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A94">
         <v>93</v>
       </c>
@@ -4146,7 +4146,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A95">
         <v>94</v>
       </c>
@@ -4181,7 +4181,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A96">
         <v>95</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A97">
         <v>96</v>
       </c>
@@ -4251,7 +4251,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A98">
         <v>97</v>
       </c>
@@ -4286,7 +4286,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A99">
         <v>98</v>
       </c>
@@ -4321,7 +4321,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A100">
         <v>99</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A101">
         <v>100</v>
       </c>
@@ -4391,7 +4391,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A102">
         <v>101</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A103">
         <v>102</v>
       </c>
@@ -4461,7 +4461,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A104">
         <v>103</v>
       </c>
@@ -4496,7 +4496,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A105">
         <v>104</v>
       </c>
@@ -4531,7 +4531,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A106">
         <v>105</v>
       </c>
@@ -4566,7 +4566,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A107">
         <v>106</v>
       </c>
@@ -4601,7 +4601,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A108">
         <v>107</v>
       </c>
@@ -4636,7 +4636,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A109">
         <v>108</v>
       </c>
@@ -4671,7 +4671,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A110">
         <v>109</v>
       </c>
@@ -4706,7 +4706,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A111">
         <v>110</v>
       </c>
@@ -4741,7 +4741,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A112">
         <v>111</v>
       </c>
@@ -4776,7 +4776,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A113">
         <v>112</v>
       </c>
@@ -4811,7 +4811,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A114">
         <v>113</v>
       </c>
@@ -4846,7 +4846,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A115">
         <v>114</v>
       </c>
@@ -4881,7 +4881,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A116">
         <v>115</v>
       </c>
@@ -4916,7 +4916,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A117">
         <v>116</v>
       </c>
@@ -4951,7 +4951,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A118">
         <v>117</v>
       </c>
@@ -4986,7 +4986,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A119">
         <v>118</v>
       </c>
@@ -5021,7 +5021,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A120">
         <v>119</v>
       </c>
@@ -5056,7 +5056,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A121">
         <v>120</v>
       </c>
@@ -5091,7 +5091,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A122">
         <v>121</v>
       </c>
@@ -5126,7 +5126,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A123">
         <v>122</v>
       </c>
@@ -5161,7 +5161,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A124">
         <v>123</v>
       </c>
@@ -5196,7 +5196,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A125">
         <v>124</v>
       </c>
@@ -5231,7 +5231,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A126">
         <v>125</v>
       </c>
@@ -5266,7 +5266,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A127">
         <v>126</v>
       </c>
@@ -5301,7 +5301,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A128">
         <v>127</v>
       </c>
@@ -5336,7 +5336,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A129">
         <v>128</v>
       </c>
@@ -5371,7 +5371,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A130">
         <v>129</v>
       </c>
@@ -5406,7 +5406,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A131">
         <v>130</v>
       </c>
@@ -5441,7 +5441,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A132">
         <v>131</v>
       </c>
@@ -5476,7 +5476,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A133">
         <v>132</v>
       </c>
@@ -5511,7 +5511,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A134">
         <v>133</v>
       </c>
@@ -5546,7 +5546,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A135">
         <v>134</v>
       </c>
@@ -5581,7 +5581,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A136">
         <v>135</v>
       </c>
@@ -5616,7 +5616,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A137">
         <v>136</v>
       </c>
@@ -5651,7 +5651,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A138">
         <v>137</v>
       </c>
@@ -5686,7 +5686,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A139">
         <v>138</v>
       </c>
@@ -5721,7 +5721,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A140">
         <v>139</v>
       </c>
@@ -5756,7 +5756,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A141">
         <v>140</v>
       </c>
@@ -5791,7 +5791,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A142">
         <v>141</v>
       </c>
@@ -5826,7 +5826,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A143">
         <v>142</v>
       </c>
@@ -5861,7 +5861,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A144">
         <v>143</v>
       </c>
@@ -5896,7 +5896,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A145">
         <v>144</v>
       </c>
@@ -5931,7 +5931,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A146">
         <v>145</v>
       </c>
@@ -5966,7 +5966,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A147">
         <v>146</v>
       </c>
@@ -6001,7 +6001,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A148">
         <v>147</v>
       </c>
@@ -6036,7 +6036,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A149">
         <v>148</v>
       </c>
@@ -6071,7 +6071,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A150">
         <v>149</v>
       </c>
@@ -6106,7 +6106,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A151">
         <v>150</v>
       </c>
@@ -6141,7 +6141,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A152">
         <v>151</v>
       </c>
@@ -6176,7 +6176,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A153">
         <v>152</v>
       </c>
@@ -6211,7 +6211,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A154">
         <v>153</v>
       </c>
@@ -6246,7 +6246,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A155">
         <v>154</v>
       </c>
@@ -6281,7 +6281,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A156">
         <v>155</v>
       </c>
@@ -6316,7 +6316,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A157">
         <v>156</v>
       </c>
@@ -6351,7 +6351,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A158">
         <v>157</v>
       </c>
@@ -6386,7 +6386,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A159">
         <v>158</v>
       </c>
@@ -6421,7 +6421,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A160">
         <v>159</v>
       </c>
@@ -6456,7 +6456,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A161">
         <v>160</v>
       </c>
@@ -6491,7 +6491,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A162">
         <v>161</v>
       </c>
@@ -6526,7 +6526,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A163">
         <v>162</v>
       </c>
@@ -6561,7 +6561,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A164">
         <v>163</v>
       </c>
@@ -6596,7 +6596,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A165">
         <v>164</v>
       </c>
@@ -6631,7 +6631,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A166">
         <v>165</v>
       </c>
@@ -6666,7 +6666,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A167">
         <v>166</v>
       </c>
@@ -6701,7 +6701,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A168">
         <v>167</v>
       </c>
@@ -6736,7 +6736,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A169">
         <v>168</v>
       </c>
@@ -6771,7 +6771,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A170">
         <v>169</v>
       </c>
@@ -6806,7 +6806,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A171">
         <v>170</v>
       </c>
@@ -6841,7 +6841,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A172">
         <v>171</v>
       </c>
@@ -6876,7 +6876,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A173">
         <v>172</v>
       </c>
@@ -6911,7 +6911,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A174">
         <v>173</v>
       </c>
@@ -6946,7 +6946,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A175">
         <v>174</v>
       </c>
@@ -6981,7 +6981,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A176">
         <v>175</v>
       </c>
@@ -7016,7 +7016,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A177">
         <v>176</v>
       </c>
@@ -7051,7 +7051,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A178">
         <v>177</v>
       </c>
@@ -7086,7 +7086,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A179">
         <v>178</v>
       </c>
@@ -7121,7 +7121,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A180">
         <v>179</v>
       </c>
@@ -7156,7 +7156,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A181">
         <v>180</v>
       </c>
@@ -7191,7 +7191,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A182">
         <v>181</v>
       </c>
@@ -7226,7 +7226,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A183">
         <v>182</v>
       </c>
@@ -7261,7 +7261,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A184">
         <v>183</v>
       </c>
@@ -7296,7 +7296,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A185">
         <v>184</v>
       </c>
@@ -7331,7 +7331,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A186">
         <v>185</v>
       </c>
@@ -7366,7 +7366,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A187">
         <v>186</v>
       </c>
@@ -7401,7 +7401,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A188">
         <v>187</v>
       </c>
@@ -7436,7 +7436,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A189">
         <v>188</v>
       </c>
@@ -7471,7 +7471,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A190">
         <v>189</v>
       </c>
@@ -7506,7 +7506,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A191">
         <v>190</v>
       </c>
@@ -7541,7 +7541,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A192">
         <v>191</v>
       </c>
@@ -7576,7 +7576,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A193">
         <v>192</v>
       </c>
@@ -7611,7 +7611,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A194">
         <v>193</v>
       </c>
@@ -7646,7 +7646,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A195">
         <v>194</v>
       </c>
@@ -7681,7 +7681,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A196">
         <v>195</v>
       </c>
@@ -7716,7 +7716,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A197">
         <v>196</v>
       </c>
@@ -7751,7 +7751,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A198">
         <v>197</v>
       </c>
@@ -7786,7 +7786,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A199">
         <v>198</v>
       </c>
@@ -7821,7 +7821,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A200">
         <v>199</v>
       </c>
@@ -7856,7 +7856,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A201">
         <v>200</v>
       </c>
@@ -7891,7 +7891,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A202">
         <v>201</v>
       </c>
@@ -7926,7 +7926,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A203">
         <v>202</v>
       </c>
@@ -7961,7 +7961,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A204">
         <v>203</v>
       </c>
@@ -7996,7 +7996,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A205">
         <v>204</v>
       </c>
@@ -8031,7 +8031,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A206">
         <v>205</v>
       </c>
@@ -8066,7 +8066,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A207">
         <v>206</v>
       </c>
@@ -8101,7 +8101,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A208">
         <v>207</v>
       </c>
@@ -8136,7 +8136,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A209">
         <v>208</v>
       </c>
@@ -8171,7 +8171,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A210">
         <v>209</v>
       </c>
@@ -8206,7 +8206,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A211">
         <v>210</v>
       </c>
@@ -8241,7 +8241,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A212">
         <v>211</v>
       </c>
@@ -8276,7 +8276,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A213">
         <v>212</v>
       </c>
@@ -8311,7 +8311,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A214">
         <v>213</v>
       </c>
@@ -8346,7 +8346,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A215">
         <v>214</v>
       </c>
@@ -8381,7 +8381,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A216">
         <v>215</v>
       </c>
@@ -8416,7 +8416,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A217">
         <v>216</v>
       </c>
@@ -8451,7 +8451,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A218">
         <v>217</v>
       </c>
@@ -8486,7 +8486,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A219">
         <v>218</v>
       </c>
@@ -8521,7 +8521,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A220">
         <v>219</v>
       </c>
@@ -8556,7 +8556,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A221">
         <v>220</v>
       </c>
@@ -8591,7 +8591,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A222">
         <v>221</v>
       </c>
@@ -8626,7 +8626,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A223">
         <v>222</v>
       </c>
@@ -8661,7 +8661,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A224">
         <v>223</v>
       </c>
@@ -8696,7 +8696,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A225">
         <v>224</v>
       </c>
@@ -8731,7 +8731,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A226">
         <v>225</v>
       </c>
@@ -8766,7 +8766,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A227">
         <v>226</v>
       </c>
@@ -8801,7 +8801,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A228">
         <v>227</v>
       </c>
@@ -8836,7 +8836,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A229">
         <v>228</v>
       </c>
@@ -8871,7 +8871,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A230">
         <v>229</v>
       </c>
@@ -8906,7 +8906,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A231">
         <v>230</v>
       </c>
@@ -8941,7 +8941,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A232">
         <v>231</v>
       </c>
@@ -8976,7 +8976,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A233">
         <v>232</v>
       </c>
@@ -9011,7 +9011,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A234">
         <v>233</v>
       </c>
@@ -9046,7 +9046,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A235">
         <v>234</v>
       </c>
@@ -9081,7 +9081,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A236">
         <v>235</v>
       </c>
@@ -9116,7 +9116,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A237">
         <v>236</v>
       </c>
@@ -9151,7 +9151,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A238">
         <v>237</v>
       </c>
@@ -9186,7 +9186,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A239">
         <v>238</v>
       </c>
@@ -9221,7 +9221,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A240">
         <v>239</v>
       </c>
@@ -9256,7 +9256,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A241">
         <v>240</v>
       </c>
@@ -9291,7 +9291,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A242">
         <v>241</v>
       </c>
@@ -9326,7 +9326,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A243">
         <v>242</v>
       </c>
@@ -9361,7 +9361,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A244">
         <v>243</v>
       </c>
@@ -9396,7 +9396,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A245">
         <v>244</v>
       </c>
@@ -9431,7 +9431,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A246">
         <v>245</v>
       </c>
@@ -9466,7 +9466,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A247">
         <v>246</v>
       </c>
@@ -9501,7 +9501,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A248">
         <v>247</v>
       </c>
@@ -9536,7 +9536,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A249">
         <v>248</v>
       </c>
@@ -9571,7 +9571,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A250">
         <v>249</v>
       </c>
@@ -9606,7 +9606,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A251">
         <v>250</v>
       </c>
@@ -9641,7 +9641,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A252">
         <v>251</v>
       </c>
@@ -9676,7 +9676,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A253">
         <v>252</v>
       </c>
@@ -9711,7 +9711,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A254">
         <v>253</v>
       </c>
@@ -9746,7 +9746,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A255">
         <v>254</v>
       </c>
@@ -9781,7 +9781,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A256">
         <v>255</v>
       </c>
@@ -9816,7 +9816,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A257">
         <v>256</v>
       </c>
@@ -9851,7 +9851,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A258">
         <v>257</v>
       </c>
@@ -9886,7 +9886,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A259">
         <v>258</v>
       </c>
@@ -9921,7 +9921,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A260">
         <v>259</v>
       </c>
@@ -9956,7 +9956,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A261">
         <v>260</v>
       </c>
@@ -9991,7 +9991,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A262">
         <v>261</v>
       </c>
@@ -10026,7 +10026,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A263">
         <v>262</v>
       </c>
@@ -10061,7 +10061,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A264">
         <v>263</v>
       </c>
@@ -10096,7 +10096,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A265">
         <v>264</v>
       </c>
@@ -10131,7 +10131,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A266">
         <v>265</v>
       </c>
@@ -10166,7 +10166,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A267">
         <v>266</v>
       </c>
@@ -10201,7 +10201,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A268">
         <v>267</v>
       </c>
@@ -10236,7 +10236,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A269">
         <v>268</v>
       </c>
@@ -10271,7 +10271,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A270">
         <v>269</v>
       </c>
@@ -10306,7 +10306,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A271">
         <v>270</v>
       </c>
@@ -10341,7 +10341,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A272">
         <v>271</v>
       </c>
@@ -10376,7 +10376,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A273">
         <v>272</v>
       </c>
@@ -10411,7 +10411,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A274">
         <v>273</v>
       </c>
@@ -10446,7 +10446,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A275">
         <v>274</v>
       </c>
@@ -10481,7 +10481,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A276">
         <v>275</v>
       </c>
@@ -10516,7 +10516,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A277">
         <v>276</v>
       </c>
@@ -10551,7 +10551,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A278">
         <v>277</v>
       </c>
@@ -10586,7 +10586,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A279">
         <v>278</v>
       </c>
@@ -10621,7 +10621,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A280">
         <v>279</v>
       </c>
@@ -10656,7 +10656,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A281">
         <v>280</v>
       </c>
@@ -10691,7 +10691,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A282">
         <v>281</v>
       </c>
@@ -10726,7 +10726,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A283">
         <v>282</v>
       </c>
@@ -10761,7 +10761,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A284">
         <v>283</v>
       </c>
@@ -10796,7 +10796,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A285">
         <v>284</v>
       </c>
@@ -10831,7 +10831,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A286">
         <v>285</v>
       </c>
@@ -10866,7 +10866,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A287">
         <v>286</v>
       </c>
@@ -10901,7 +10901,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A288">
         <v>287</v>
       </c>
@@ -10936,7 +10936,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A289">
         <v>288</v>
       </c>
@@ -10971,7 +10971,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A290">
         <v>289</v>
       </c>
@@ -11006,7 +11006,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A291">
         <v>290</v>
       </c>
@@ -11041,7 +11041,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A292">
         <v>291</v>
       </c>
@@ -11076,7 +11076,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="293" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A293">
         <v>292</v>
       </c>
@@ -11111,7 +11111,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A294">
         <v>293</v>
       </c>
@@ -11146,7 +11146,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A295">
         <v>294</v>
       </c>
@@ -11181,7 +11181,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="296" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A296">
         <v>295</v>
       </c>
@@ -11216,7 +11216,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="297" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A297">
         <v>296</v>
       </c>
@@ -11251,7 +11251,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="298" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A298">
         <v>297</v>
       </c>
@@ -11286,7 +11286,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A299">
         <v>298</v>
       </c>
@@ -11321,7 +11321,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="300" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A300">
         <v>299</v>
       </c>
@@ -11356,7 +11356,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="301" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A301">
         <v>300</v>
       </c>
@@ -11391,7 +11391,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="302" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A302">
         <v>301</v>
       </c>
@@ -11426,7 +11426,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="303" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A303">
         <v>302</v>
       </c>
@@ -11461,7 +11461,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="304" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A304">
         <v>303</v>
       </c>
@@ -11496,7 +11496,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="305" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A305">
         <v>304</v>
       </c>
@@ -11531,7 +11531,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="306" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A306">
         <v>305</v>
       </c>
@@ -11566,7 +11566,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="307" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A307">
         <v>306</v>
       </c>
@@ -11601,7 +11601,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="308" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A308">
         <v>307</v>
       </c>
@@ -11636,7 +11636,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="309" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A309">
         <v>308</v>
       </c>
@@ -11671,7 +11671,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="310" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A310">
         <v>309</v>
       </c>
@@ -11706,7 +11706,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="311" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A311">
         <v>310</v>
       </c>
@@ -11741,7 +11741,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="312" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A312">
         <v>311</v>
       </c>
@@ -11776,7 +11776,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="313" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A313">
         <v>312</v>
       </c>
@@ -11811,7 +11811,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="314" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A314">
         <v>313</v>
       </c>
@@ -11846,7 +11846,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="315" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A315">
         <v>314</v>
       </c>
@@ -11881,7 +11881,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="316" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A316">
         <v>315</v>
       </c>
@@ -11916,7 +11916,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="317" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A317">
         <v>316</v>
       </c>
@@ -11951,7 +11951,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="318" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A318">
         <v>317</v>
       </c>
@@ -11986,7 +11986,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="319" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A319">
         <v>318</v>
       </c>
@@ -12021,7 +12021,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="320" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A320">
         <v>319</v>
       </c>
@@ -12056,7 +12056,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="321" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A321">
         <v>320</v>
       </c>
@@ -12091,7 +12091,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="322" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A322">
         <v>321</v>
       </c>
@@ -12126,7 +12126,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="323" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A323">
         <v>322</v>
       </c>
@@ -12161,7 +12161,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="324" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A324">
         <v>323</v>
       </c>
@@ -12196,7 +12196,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="325" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A325">
         <v>324</v>
       </c>
@@ -12231,7 +12231,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="326" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A326">
         <v>325</v>
       </c>
@@ -12266,7 +12266,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="327" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A327">
         <v>326</v>
       </c>
@@ -12301,7 +12301,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="328" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A328">
         <v>327</v>
       </c>
@@ -12336,7 +12336,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="329" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A329">
         <v>328</v>
       </c>
@@ -12371,7 +12371,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="330" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A330">
         <v>329</v>
       </c>
@@ -12406,7 +12406,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="331" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A331">
         <v>330</v>
       </c>
@@ -12441,7 +12441,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="332" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A332">
         <v>331</v>
       </c>
@@ -12476,7 +12476,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="333" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A333">
         <v>332</v>
       </c>
@@ -12511,7 +12511,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="334" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A334">
         <v>333</v>
       </c>
@@ -12546,7 +12546,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="335" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A335">
         <v>334</v>
       </c>
@@ -12581,7 +12581,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="336" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A336">
         <v>335</v>
       </c>
@@ -12616,7 +12616,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="337" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A337">
         <v>336</v>
       </c>
@@ -12651,7 +12651,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="338" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A338">
         <v>337</v>
       </c>
@@ -12686,7 +12686,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="339" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A339">
         <v>338</v>
       </c>
@@ -12721,7 +12721,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="340" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A340">
         <v>339</v>
       </c>
@@ -12756,7 +12756,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="341" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A341">
         <v>340</v>
       </c>
@@ -12791,7 +12791,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="342" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A342">
         <v>341</v>
       </c>
@@ -12826,7 +12826,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="343" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A343">
         <v>342</v>
       </c>
@@ -12861,7 +12861,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="344" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A344">
         <v>343</v>
       </c>
@@ -12896,7 +12896,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="345" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A345">
         <v>344</v>
       </c>
@@ -12931,7 +12931,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="346" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A346">
         <v>345</v>
       </c>
@@ -12966,7 +12966,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="347" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A347">
         <v>346</v>
       </c>
@@ -13001,7 +13001,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="348" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A348">
         <v>347</v>
       </c>
@@ -13036,7 +13036,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="349" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A349">
         <v>348</v>
       </c>
@@ -13071,7 +13071,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="350" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A350">
         <v>349</v>
       </c>
@@ -13106,7 +13106,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="351" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A351">
         <v>350</v>
       </c>
@@ -13141,7 +13141,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="352" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A352">
         <v>351</v>
       </c>
@@ -13176,7 +13176,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="353" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A353">
         <v>352</v>
       </c>
@@ -13211,7 +13211,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="354" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A354">
         <v>353</v>
       </c>
@@ -13246,7 +13246,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="355" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A355">
         <v>354</v>
       </c>
@@ -13281,7 +13281,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="356" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A356">
         <v>355</v>
       </c>
@@ -13316,7 +13316,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="357" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A357">
         <v>356</v>
       </c>
@@ -13351,7 +13351,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="358" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A358">
         <v>357</v>
       </c>
@@ -13386,7 +13386,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="359" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A359">
         <v>358</v>
       </c>
@@ -13421,7 +13421,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="360" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A360">
         <v>359</v>
       </c>
@@ -13456,7 +13456,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="361" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A361">
         <v>360</v>
       </c>
@@ -13491,7 +13491,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="362" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A362">
         <v>361</v>
       </c>
@@ -13526,7 +13526,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="363" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A363">
         <v>362</v>
       </c>
@@ -13561,7 +13561,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="364" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A364">
         <v>363</v>
       </c>
@@ -13596,7 +13596,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="365" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A365">
         <v>364</v>
       </c>
@@ -13631,7 +13631,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="366" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A366">
         <v>365</v>
       </c>
@@ -13666,7 +13666,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="367" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A367">
         <v>366</v>
       </c>
@@ -13701,7 +13701,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="368" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A368">
         <v>367</v>
       </c>
@@ -13736,7 +13736,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="369" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A369">
         <v>368</v>
       </c>
@@ -13771,7 +13771,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="370" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A370">
         <v>369</v>
       </c>
@@ -13806,7 +13806,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="371" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A371">
         <v>370</v>
       </c>
@@ -13841,7 +13841,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="372" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A372">
         <v>371</v>
       </c>
@@ -13876,7 +13876,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="373" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A373">
         <v>372</v>
       </c>
@@ -13911,7 +13911,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="374" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A374">
         <v>373</v>
       </c>
@@ -13946,7 +13946,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="375" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A375">
         <v>374</v>
       </c>
@@ -13981,7 +13981,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="376" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A376">
         <v>375</v>
       </c>
@@ -14016,7 +14016,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="377" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A377">
         <v>376</v>
       </c>
@@ -14051,7 +14051,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="378" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A378">
         <v>377</v>
       </c>
@@ -14086,7 +14086,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="379" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A379">
         <v>378</v>
       </c>
@@ -14121,7 +14121,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="380" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A380">
         <v>379</v>
       </c>
@@ -14156,7 +14156,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="381" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A381">
         <v>380</v>
       </c>
@@ -14191,7 +14191,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="382" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A382">
         <v>381</v>
       </c>
@@ -14226,7 +14226,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="383" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A383">
         <v>382</v>
       </c>
@@ -14261,7 +14261,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="384" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A384">
         <v>383</v>
       </c>
@@ -14296,7 +14296,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="385" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A385">
         <v>384</v>
       </c>
@@ -14331,7 +14331,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="386" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A386">
         <v>385</v>
       </c>
@@ -14366,7 +14366,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="387" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A387">
         <v>386</v>
       </c>
@@ -14401,7 +14401,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="388" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A388">
         <v>387</v>
       </c>
@@ -14436,7 +14436,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="389" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A389">
         <v>388</v>
       </c>
@@ -14471,7 +14471,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="390" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A390">
         <v>389</v>
       </c>
@@ -14506,7 +14506,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="391" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A391">
         <v>390</v>
       </c>
@@ -14541,7 +14541,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="392" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A392">
         <v>391</v>
       </c>
@@ -14576,7 +14576,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="393" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A393">
         <v>392</v>
       </c>
@@ -14611,7 +14611,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="394" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A394">
         <v>393</v>
       </c>
@@ -14646,7 +14646,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="395" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A395">
         <v>394</v>
       </c>
@@ -14681,7 +14681,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="396" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A396">
         <v>395</v>
       </c>
@@ -14716,7 +14716,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="397" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A397">
         <v>396</v>
       </c>
@@ -14751,7 +14751,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="398" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A398">
         <v>397</v>
       </c>
@@ -14786,7 +14786,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="399" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A399">
         <v>398</v>
       </c>
@@ -14821,7 +14821,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="400" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A400">
         <v>399</v>
       </c>
@@ -14856,7 +14856,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="401" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A401">
         <v>400</v>
       </c>
@@ -14891,7 +14891,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="402" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A402">
         <v>401</v>
       </c>
@@ -14926,7 +14926,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="403" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A403">
         <v>402</v>
       </c>
@@ -14961,7 +14961,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="404" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A404">
         <v>403</v>
       </c>
@@ -14996,7 +14996,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="405" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A405">
         <v>404</v>
       </c>
@@ -15031,7 +15031,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="406" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A406">
         <v>405</v>
       </c>
@@ -15066,7 +15066,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="407" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A407">
         <v>406</v>
       </c>
@@ -15101,7 +15101,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="408" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A408">
         <v>407</v>
       </c>
@@ -15136,7 +15136,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="409" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A409">
         <v>408</v>
       </c>
@@ -15171,7 +15171,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="410" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A410">
         <v>409</v>
       </c>
@@ -15206,7 +15206,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="411" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A411">
         <v>410</v>
       </c>
@@ -15241,7 +15241,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="412" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A412">
         <v>411</v>
       </c>
@@ -15276,7 +15276,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="413" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A413">
         <v>412</v>
       </c>
@@ -15311,7 +15311,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="414" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A414">
         <v>413</v>
       </c>
@@ -15346,7 +15346,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="415" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A415">
         <v>414</v>
       </c>
@@ -15381,7 +15381,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="416" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A416">
         <v>415</v>
       </c>
@@ -15416,7 +15416,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="417" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A417">
         <v>416</v>
       </c>
@@ -15451,7 +15451,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="418" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A418">
         <v>417</v>
       </c>
@@ -15486,7 +15486,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="419" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A419">
         <v>418</v>
       </c>
@@ -15521,7 +15521,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="420" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A420">
         <v>419</v>
       </c>
@@ -15556,7 +15556,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="421" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A421">
         <v>420</v>
       </c>
@@ -15591,7 +15591,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="422" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A422">
         <v>421</v>
       </c>
@@ -15626,7 +15626,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="423" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A423">
         <v>422</v>
       </c>
@@ -15661,7 +15661,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="424" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A424">
         <v>423</v>
       </c>
@@ -15696,7 +15696,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="425" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A425">
         <v>424</v>
       </c>
@@ -15731,7 +15731,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="426" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A426">
         <v>425</v>
       </c>
@@ -15766,7 +15766,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="427" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A427">
         <v>426</v>
       </c>
@@ -15801,7 +15801,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="428" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A428">
         <v>427</v>
       </c>
@@ -15836,7 +15836,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="429" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A429">
         <v>428</v>
       </c>
@@ -15871,7 +15871,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="430" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A430">
         <v>429</v>
       </c>
@@ -15906,7 +15906,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="431" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A431">
         <v>430</v>
       </c>
@@ -15941,7 +15941,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="432" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A432">
         <v>431</v>
       </c>
@@ -15976,7 +15976,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="433" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A433">
         <v>432</v>
       </c>
@@ -16011,7 +16011,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="434" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A434">
         <v>433</v>
       </c>
@@ -16046,7 +16046,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="435" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A435">
         <v>434</v>
       </c>
@@ -16081,7 +16081,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="436" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A436">
         <v>435</v>
       </c>
@@ -16116,7 +16116,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="437" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A437">
         <v>436</v>
       </c>
@@ -16151,7 +16151,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="438" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A438">
         <v>437</v>
       </c>
@@ -16186,7 +16186,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="439" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A439">
         <v>438</v>
       </c>
@@ -16221,7 +16221,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="440" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A440">
         <v>439</v>
       </c>
@@ -16256,7 +16256,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="441" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A441">
         <v>440</v>
       </c>
@@ -16291,7 +16291,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="442" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A442">
         <v>441</v>
       </c>
@@ -16326,7 +16326,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="443" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A443">
         <v>442</v>
       </c>
@@ -16361,7 +16361,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="444" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A444">
         <v>443</v>
       </c>
@@ -16396,7 +16396,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="445" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A445">
         <v>444</v>
       </c>
@@ -16431,7 +16431,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="446" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A446">
         <v>445</v>
       </c>
@@ -16466,7 +16466,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="447" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A447">
         <v>446</v>
       </c>
@@ -16501,7 +16501,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="448" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A448">
         <v>447</v>
       </c>
@@ -16536,7 +16536,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="449" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A449">
         <v>448</v>
       </c>
@@ -16571,7 +16571,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="450" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A450">
         <v>449</v>
       </c>
@@ -16606,7 +16606,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="451" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A451">
         <v>450</v>
       </c>
@@ -16641,7 +16641,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="452" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A452">
         <v>451</v>
       </c>
@@ -16676,7 +16676,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="453" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A453">
         <v>452</v>
       </c>
@@ -16711,7 +16711,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="454" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A454">
         <v>453</v>
       </c>
@@ -16746,7 +16746,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="455" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A455">
         <v>454</v>
       </c>
@@ -16781,7 +16781,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="456" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A456">
         <v>455</v>
       </c>
@@ -16816,7 +16816,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="457" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A457">
         <v>456</v>
       </c>
@@ -16851,7 +16851,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="458" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A458">
         <v>457</v>
       </c>
@@ -16886,7 +16886,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="459" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A459">
         <v>458</v>
       </c>
@@ -16921,7 +16921,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="460" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A460">
         <v>459</v>
       </c>
@@ -16956,7 +16956,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="461" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A461">
         <v>460</v>
       </c>
@@ -16991,7 +16991,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="462" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A462">
         <v>461</v>
       </c>
@@ -17026,7 +17026,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="463" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A463">
         <v>462</v>
       </c>
@@ -17061,7 +17061,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="464" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A464">
         <v>463</v>
       </c>
@@ -17096,7 +17096,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="465" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A465">
         <v>464</v>
       </c>
@@ -17131,7 +17131,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="466" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A466">
         <v>465</v>
       </c>
@@ -17166,7 +17166,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="467" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A467">
         <v>466</v>
       </c>
@@ -17201,7 +17201,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="468" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A468">
         <v>467</v>
       </c>
@@ -17236,7 +17236,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="469" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A469">
         <v>468</v>
       </c>
@@ -17271,7 +17271,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="470" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A470">
         <v>469</v>
       </c>
@@ -17306,7 +17306,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="471" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A471">
         <v>470</v>
       </c>
@@ -17341,7 +17341,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="472" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A472">
         <v>471</v>
       </c>
@@ -17376,7 +17376,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="473" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A473">
         <v>472</v>
       </c>
@@ -17411,7 +17411,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="474" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A474">
         <v>473</v>
       </c>
@@ -17446,7 +17446,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="475" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A475">
         <v>474</v>
       </c>
@@ -17481,7 +17481,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="476" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A476">
         <v>475</v>
       </c>
@@ -17516,7 +17516,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="477" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A477">
         <v>476</v>
       </c>
@@ -17551,7 +17551,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="478" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A478">
         <v>477</v>
       </c>
@@ -17586,7 +17586,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="479" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A479">
         <v>478</v>
       </c>
@@ -17621,7 +17621,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="480" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A480">
         <v>479</v>
       </c>
@@ -17656,7 +17656,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="481" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A481">
         <v>480</v>
       </c>
@@ -17691,7 +17691,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="482" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A482">
         <v>481</v>
       </c>
@@ -17726,7 +17726,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="483" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A483">
         <v>482</v>
       </c>
@@ -17761,7 +17761,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="484" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A484">
         <v>483</v>
       </c>
@@ -17796,7 +17796,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="485" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A485">
         <v>484</v>
       </c>
@@ -17831,7 +17831,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="486" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A486">
         <v>485</v>
       </c>
@@ -17866,7 +17866,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="487" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A487">
         <v>486</v>
       </c>
@@ -17901,7 +17901,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="488" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A488">
         <v>487</v>
       </c>
@@ -17936,7 +17936,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="489" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="489" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A489">
         <v>488</v>
       </c>
@@ -17971,7 +17971,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="490" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="490" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A490">
         <v>489</v>
       </c>
@@ -18006,7 +18006,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="491" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="491" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A491">
         <v>490</v>
       </c>
@@ -18041,7 +18041,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="492" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A492">
         <v>491</v>
       </c>
@@ -18076,7 +18076,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="493" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="493" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A493">
         <v>492</v>
       </c>
@@ -18111,7 +18111,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="494" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="494" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A494">
         <v>493</v>
       </c>
@@ -18146,7 +18146,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="495" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="495" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A495">
         <v>494</v>
       </c>
@@ -18181,7 +18181,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="496" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="496" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A496">
         <v>495</v>
       </c>
@@ -18216,7 +18216,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="497" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A497">
         <v>496</v>
       </c>
@@ -18251,7 +18251,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="498" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="498" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A498">
         <v>497</v>
       </c>
@@ -18286,7 +18286,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="499" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="499" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A499">
         <v>498</v>
       </c>
@@ -18321,7 +18321,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="500" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="500" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A500">
         <v>499</v>
       </c>
@@ -18356,7 +18356,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="501" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="501" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A501">
         <v>500</v>
       </c>

</xml_diff>